<commit_message>
fix impl. H-Count error on pharmacophore generation
</commit_message>
<xml_diff>
--- a/scripts/targets/Tubulin_Colchicine_domain.xlsx
+++ b/scripts/targets/Tubulin_Colchicine_domain.xlsx
@@ -52,6 +52,27 @@
     <t xml:space="preserve">Target_system</t>
   </si>
   <si>
+    <t xml:space="preserve">COc1c(OC)cc(cc1OC)[C@H]1[C@H]2C(=O)OC[C@H]2[C@H](c2c1cc1OCOc1c2)Sc1[nH]ncn1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5jcb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NV4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTP,ACP,GDP,MES,GOL,IMD,CA,Mg,NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=</t>
+  </si>
+  <si>
     <t xml:space="preserve">CO[C@H]1CC[C@H]2[C@@H](CC1=O)[C@H](CCc1c2c(OC)c(c(c1)OC)OC)NC(=O)C</t>
   </si>
   <si>
@@ -64,28 +85,7 @@
     <t xml:space="preserve">MES,GOL,GTP,GDP.CA,Mg</t>
   </si>
   <si>
-    <t xml:space="preserve">nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tubulin-colchicine binding domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COc1c(OC)cc(cc1OC)[C@H]1[C@H]2C(=O)OC[C@H]2[C@H](c2c1cc1OCOc1c2)Sc1[nH]ncn1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5jcb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NV4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTP,ACP,GDP,MES,GOL,IMD,CA,Mg,NA</t>
   </si>
   <si>
     <t xml:space="preserve">COc1c2c(CC[C@H](c3c2ccc(c(=O)c3)SC)NC(=O)C)cc(c1OC)OC</t>
@@ -261,13 +261,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.86"/>
   </cols>
@@ -306,7 +306,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>10</v>
@@ -330,27 +330,24 @@
         <v>16</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>11030</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>62040</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>14</v>
@@ -362,7 +359,10 @@
         <v>16</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>62040</v>
+        <v>11030</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,7 +553,7 @@
         <v>47</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>14</v>
@@ -568,6 +568,7 @@
         <v>2500</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>